<commit_message>
Pulir CV Uniandes 2023
</commit_message>
<xml_diff>
--- a/Especial_Uniandes_2023/data/grant_es.xlsx
+++ b/Especial_Uniandes_2023/data/grant_es.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1DC8D-B3FA-450B-A321-B42B16290506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D60CBA9-8861-4732-A30D-2C251598C8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>

</xml_diff>